<commit_message>
fixed timestep bug and window size
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond_Stat.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond_Stat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -230,7 +230,7 @@
     <t xml:space="preserve"> Beta Lipid Omn (default = 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Beta Non-lipid OM (defualt = 0.035)</t>
+    <t xml:space="preserve">Beta Non-lipid OM (default = 0.035)</t>
   </si>
   <si>
     <t xml:space="preserve">Beta Lipid digesta (default = 1)</t>
@@ -239,7 +239,7 @@
     <t xml:space="preserve">Beta Sediment OC (default = .35)</t>
   </si>
   <si>
-    <t xml:space="preserve">Beta  Non-lipid digesta  (defualt = .035)</t>
+    <t xml:space="preserve">Beta  Non-lipid digesta  (default = .035)</t>
   </si>
   <si>
     <t xml:space="preserve">PCB 52</t>
@@ -1287,9 +1287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1017720</xdr:colOff>
+      <xdr:colOff>1017000</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1299,7 +1299,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14045040" y="571680"/>
-          <a:ext cx="9469800" cy="7807680"/>
+          <a:ext cx="9469080" cy="7806960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1766,9 +1766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2968560</xdr:colOff>
+      <xdr:colOff>2967840</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1778,7 +1778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11978640" y="546120"/>
-          <a:ext cx="2968560" cy="569160"/>
+          <a:ext cx="2967840" cy="568440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1989,9 +1989,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>5213520</xdr:colOff>
+      <xdr:colOff>5212800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2001,7 +2001,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="2464920"/>
-          <a:ext cx="9910800" cy="4177080"/>
+          <a:ext cx="9910080" cy="4176360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2300,9 +2300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2329920</xdr:colOff>
+      <xdr:colOff>2329200</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2316,7 +2316,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2329920" cy="734040"/>
+          <a:ext cx="2329200" cy="733320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2477,9 +2477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2489,7 +2489,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22839480" y="2082960"/>
-          <a:ext cx="3746520" cy="759240"/>
+          <a:ext cx="3745800" cy="758520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2619,9 +2619,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1017360</xdr:colOff>
+      <xdr:colOff>1016640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2631,7 +2631,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21425760" y="2130480"/>
-          <a:ext cx="2878920" cy="759240"/>
+          <a:ext cx="2878200" cy="758520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2973,9 +2973,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2985,7 +2985,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15024240" y="594720"/>
-          <a:ext cx="4076280" cy="950400"/>
+          <a:ext cx="4075560" cy="949680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3042,9 +3042,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>897480</xdr:colOff>
+      <xdr:colOff>896760</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3054,7 +3054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14243040" y="3772800"/>
-          <a:ext cx="9086760" cy="3477240"/>
+          <a:ext cx="9086040" cy="3476520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3502,7 +3502,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>644400</xdr:colOff>
+      <xdr:colOff>643680</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>188640</xdr:rowOff>
     </xdr:to>
@@ -3514,7 +3514,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5642280" y="9319320"/>
-          <a:ext cx="8330040" cy="650520"/>
+          <a:ext cx="8329320" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3672,9 +3672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4549680</xdr:colOff>
+      <xdr:colOff>4548960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3684,7 +3684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11780280" y="3467880"/>
-          <a:ext cx="4061520" cy="747720"/>
+          <a:ext cx="4060800" cy="747000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3786,9 +3786,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4614120</xdr:colOff>
+      <xdr:colOff>4613400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3798,7 +3798,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17375400" y="3725640"/>
-          <a:ext cx="4330800" cy="340200"/>
+          <a:ext cx="4330080" cy="339480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3915,9 +3915,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5382360</xdr:colOff>
+      <xdr:colOff>5381640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3927,7 +3927,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5255280" cy="1495800"/>
+          <a:ext cx="5254560" cy="1495080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4129,9 +4129,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4988880</xdr:colOff>
+      <xdr:colOff>4988160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4141,7 +4141,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12084120" y="2705040"/>
-          <a:ext cx="1991520" cy="658080"/>
+          <a:ext cx="1990800" cy="657360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4248,9 +4248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>759600</xdr:colOff>
+      <xdr:colOff>758880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4260,7 +4260,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11168280" y="4140000"/>
-          <a:ext cx="10732680" cy="390960"/>
+          <a:ext cx="10731960" cy="390240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4372,9 +4372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4384,7 +4384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12163680" y="2984400"/>
-          <a:ext cx="9178200" cy="416520"/>
+          <a:ext cx="9177480" cy="415800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4441,9 +4441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>531000</xdr:colOff>
+      <xdr:colOff>530280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4453,7 +4453,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12151080" y="3556080"/>
-          <a:ext cx="11886120" cy="695880"/>
+          <a:ext cx="11885400" cy="695160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4515,9 +4515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>276840</xdr:colOff>
+      <xdr:colOff>276120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4527,7 +4527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899600" y="762120"/>
-          <a:ext cx="6528960" cy="5942520"/>
+          <a:ext cx="6528240" cy="5941800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4643,8 +4643,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="D1" s="3" t="n">
         <f aca="false">B2*B3</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4674,7 +4674,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -4684,7 +4684,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -4694,7 +4694,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -4762,7 +4762,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5537,8 +5537,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11503,7 +11503,7 @@
   </sheetPr>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added manual, and found and fixed phyto bug
</commit_message>
<xml_diff>
--- a/sheets/input/Pegan_Cove_South_Pond_Stat.xlsx
+++ b/sheets/input/Pegan_Cove_South_Pond_Stat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -105,10 +105,10 @@
     <t xml:space="preserve">Dissolved oxygen concentration (if avaliable) (mg O2/L)</t>
   </si>
   <si>
-    <t xml:space="preserve">POC–octanol proportionality constant (only if Cwdo is unavaliable) (deafult if not entered = .08)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOC–octanol proportionality constant(only if Cwdo is unavaliable) (deafult if note entered = .35)</t>
+    <t xml:space="preserve">POC–octanol proportionality constant (only if Cwdo is unavaliable) (deafult if not entered = .35)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC–octanol proportionality constant(only if Cwdo is unavaliable) (deafult if note entered = .08)</t>
   </si>
   <si>
     <t xml:space="preserve">Pegan Cove dummy</t>
@@ -521,10 +521,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -920,7 +921,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -940,7 +941,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,7 +965,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1044,7 +1045,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1064,7 +1065,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1076,7 +1077,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1084,7 +1085,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1124,7 +1125,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1156,7 +1157,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1287,9 +1288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1017000</xdr:colOff>
+      <xdr:colOff>1016640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1299,7 +1300,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14045040" y="571680"/>
-          <a:ext cx="9469080" cy="7806960"/>
+          <a:ext cx="9468720" cy="7806600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1766,9 +1767,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2967840</xdr:colOff>
+      <xdr:colOff>2967480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1778,7 +1779,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11978640" y="546120"/>
-          <a:ext cx="2967840" cy="568440"/>
+          <a:ext cx="2967480" cy="568080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1989,9 +1990,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>5212800</xdr:colOff>
+      <xdr:colOff>5212440</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2001,7 +2002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11979000" y="2464920"/>
-          <a:ext cx="9910080" cy="4176360"/>
+          <a:ext cx="9909720" cy="4176000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2300,9 +2301,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2329200</xdr:colOff>
+      <xdr:colOff>2328840</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2316,7 +2317,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2329200" cy="733320"/>
+          <a:ext cx="2328840" cy="732960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2477,9 +2478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>238680</xdr:colOff>
+      <xdr:colOff>238320</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2489,7 +2490,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22839480" y="2082960"/>
-          <a:ext cx="3745800" cy="758520"/>
+          <a:ext cx="3745440" cy="758160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2619,9 +2620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1016640</xdr:colOff>
+      <xdr:colOff>1016280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2631,7 +2632,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21425760" y="2130480"/>
-          <a:ext cx="2878200" cy="758520"/>
+          <a:ext cx="2877840" cy="758160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2973,9 +2974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2985,7 +2986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15024240" y="594720"/>
-          <a:ext cx="4075560" cy="949680"/>
+          <a:ext cx="4075200" cy="949320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3042,9 +3043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>896760</xdr:colOff>
+      <xdr:colOff>896400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3054,7 +3055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14243040" y="3772800"/>
-          <a:ext cx="9086040" cy="3476520"/>
+          <a:ext cx="9085680" cy="3476160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3502,7 +3503,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>643680</xdr:colOff>
+      <xdr:colOff>643320</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>188640</xdr:rowOff>
     </xdr:to>
@@ -3514,7 +3515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5642280" y="9319320"/>
-          <a:ext cx="8329320" cy="650520"/>
+          <a:ext cx="8328960" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3672,9 +3673,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4548960</xdr:colOff>
+      <xdr:colOff>4548600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3684,7 +3685,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11780280" y="3467880"/>
-          <a:ext cx="4060800" cy="747000"/>
+          <a:ext cx="4060440" cy="746640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3786,9 +3787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4613400</xdr:colOff>
+      <xdr:colOff>4613040</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3798,7 +3799,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17375400" y="3725640"/>
-          <a:ext cx="4330080" cy="339480"/>
+          <a:ext cx="4329720" cy="339120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3915,9 +3916,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5381640</xdr:colOff>
+      <xdr:colOff>5381280</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3927,7 +3928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5254560" cy="1495080"/>
+          <a:ext cx="5254200" cy="1494720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4129,9 +4130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4988160</xdr:colOff>
+      <xdr:colOff>4987800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4141,7 +4142,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12084120" y="2705040"/>
-          <a:ext cx="1990800" cy="657360"/>
+          <a:ext cx="1990440" cy="657000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4248,9 +4249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>758880</xdr:colOff>
+      <xdr:colOff>758520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4260,7 +4261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11168280" y="4140000"/>
-          <a:ext cx="10731960" cy="390240"/>
+          <a:ext cx="10731600" cy="389880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4372,9 +4373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>199800</xdr:colOff>
+      <xdr:colOff>199440</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4384,7 +4385,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12163680" y="2984400"/>
-          <a:ext cx="9177480" cy="415800"/>
+          <a:ext cx="9177120" cy="415440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4441,9 +4442,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>530280</xdr:colOff>
+      <xdr:colOff>529920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4453,7 +4454,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12151080" y="3556080"/>
-          <a:ext cx="11885400" cy="695160"/>
+          <a:ext cx="11885040" cy="694800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4515,9 +4516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>276120</xdr:colOff>
+      <xdr:colOff>275760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4527,7 +4528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899600" y="762120"/>
-          <a:ext cx="6528240" cy="5941800"/>
+          <a:ext cx="6527880" cy="5941440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4644,7 +4645,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="A39:A40 A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4761,8 +4762,8 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5185,7 +5186,7 @@
   <dimension ref="A1:BI5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A39:A40 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5537,8 +5538,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="A39:A40 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5725,7 +5726,7 @@
   <dimension ref="A1:BJ46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A39:A40 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9587,7 +9588,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="A39:A40 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10068,7 +10069,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="A39:A40 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10316,7 +10317,7 @@
   <dimension ref="A1:TL4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
+      <selection pane="topLeft" activeCell="AB1" activeCellId="1" sqref="A39:A40 AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11504,7 +11505,7 @@
   <dimension ref="A1:AW100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="A39:A40 A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>